<commit_message>
additionally check for correct country/city combination
</commit_message>
<xml_diff>
--- a/dummy_data.xlsx
+++ b/dummy_data.xlsx
@@ -1,10 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24332"/>
+  <workbookPr filterPrivacy="1"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44A3B9E8-EBC9-49B6-85A8-6824D2BE35AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="-105" windowWidth="19305" windowHeight="7170"/>
+    <workbookView xWindow="9330" yWindow="19890" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -12,17 +13,26 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Tabelle1!$A$1:$C$9078</definedName>
   </definedNames>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="897" uniqueCount="187">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="897" uniqueCount="184">
   <si>
     <t>Lnd</t>
   </si>
@@ -55,9 +65,6 @@
   </si>
   <si>
     <t>JP</t>
-  </si>
-  <si>
-    <t>Japan Tokio</t>
   </si>
   <si>
     <t>Düsseldorf</t>
@@ -417,9 +424,6 @@
     <t>Datteln</t>
   </si>
   <si>
-    <t>Alba</t>
-  </si>
-  <si>
     <t>Paris</t>
   </si>
   <si>
@@ -540,9 +544,6 @@
     <t>Lünen</t>
   </si>
   <si>
-    <t>Marl</t>
-  </si>
-  <si>
     <t>Fellbach</t>
   </si>
   <si>
@@ -564,18 +565,6 @@
     <t xml:space="preserve">Feldberg </t>
   </si>
   <si>
-    <t xml:space="preserve">Polen </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Frankreich </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Indien </t>
-  </si>
-  <si>
-    <t>Castanheira</t>
-  </si>
-  <si>
     <t>Bandung City</t>
   </si>
   <si>
@@ -584,11 +573,23 @@
   <si>
     <t>Paestum</t>
   </si>
+  <si>
+    <t>Alba Cuneo</t>
+  </si>
+  <si>
+    <t>Castanheira de Pêra</t>
+  </si>
+  <si>
+    <t>Indien</t>
+  </si>
+  <si>
+    <t>Recklinghausen</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -945,11 +946,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C11407"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+    <sheetView tabSelected="1" topLeftCell="A210" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="C225" sqref="C225"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.28515625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -968,7 +969,7 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
     </row>
     <row r="2" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -987,10 +988,10 @@
         <v>6</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="4" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -1012,7 +1013,7 @@
         <v>4</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="6" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -1056,7 +1057,7 @@
         <v>4</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="10" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -1067,29 +1068,29 @@
         <v>8</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
     </row>
     <row r="11" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B11" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="B11" s="2" t="s">
-        <v>17</v>
-      </c>
       <c r="C11" s="2" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
     </row>
     <row r="12" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B12" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="B12" s="2" t="s">
+      <c r="C12" s="2" t="s">
         <v>14</v>
-      </c>
-      <c r="C12" s="2" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="13" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -1100,7 +1101,7 @@
         <v>4</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="14" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -1111,7 +1112,7 @@
         <v>4</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="15" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -1133,7 +1134,7 @@
         <v>4</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="17" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -1144,7 +1145,7 @@
         <v>4</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="18" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -1155,7 +1156,7 @@
         <v>4</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="19" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -1163,10 +1164,10 @@
         <v>10</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>11</v>
+        <v>131</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
     </row>
     <row r="20" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -1177,7 +1178,7 @@
         <v>4</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="21" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -1188,7 +1189,7 @@
         <v>4</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="22" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -1199,7 +1200,7 @@
         <v>4</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="23" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -1210,51 +1211,51 @@
         <v>8</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
     </row>
     <row r="24" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B24" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="B24" s="2" t="s">
+      <c r="C24" s="2" t="s">
         <v>32</v>
-      </c>
-      <c r="C24" s="2" t="s">
-        <v>33</v>
       </c>
     </row>
     <row r="25" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B25" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="B25" s="2" t="s">
-        <v>17</v>
-      </c>
       <c r="C25" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="26" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B26" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="B26" s="2" t="s">
+      <c r="C26" s="2" t="s">
         <v>28</v>
-      </c>
-      <c r="C26" s="2" t="s">
-        <v>29</v>
       </c>
     </row>
     <row r="27" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B27" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="B27" s="2" t="s">
-        <v>26</v>
-      </c>
       <c r="C27" s="2" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
     </row>
     <row r="28" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -1265,7 +1266,7 @@
         <v>4</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="29" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -1276,18 +1277,18 @@
         <v>8</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="30" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B30" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="B30" s="2" t="s">
+      <c r="C30" s="2" t="s">
         <v>21</v>
-      </c>
-      <c r="C30" s="2" t="s">
-        <v>22</v>
       </c>
     </row>
     <row r="31" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -1298,7 +1299,7 @@
         <v>4</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="32" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -1309,7 +1310,7 @@
         <v>4</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="33" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -1320,18 +1321,18 @@
         <v>4</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
     </row>
     <row r="34" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A34" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B34" s="2" t="s">
         <v>182</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>185</v>
+        <v>178</v>
       </c>
     </row>
     <row r="35" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -1342,7 +1343,7 @@
         <v>4</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="36" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -1353,7 +1354,7 @@
         <v>4</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="37" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -1364,7 +1365,7 @@
         <v>4</v>
       </c>
       <c r="C37" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="38" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -1375,7 +1376,7 @@
         <v>4</v>
       </c>
       <c r="C38" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="39" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -1386,7 +1387,7 @@
         <v>4</v>
       </c>
       <c r="C39" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="40" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -1397,7 +1398,7 @@
         <v>4</v>
       </c>
       <c r="C40" s="2" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="41" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -1408,7 +1409,7 @@
         <v>4</v>
       </c>
       <c r="C41" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="42" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -1419,18 +1420,18 @@
         <v>4</v>
       </c>
       <c r="C42" s="2" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
     </row>
     <row r="43" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A43" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="B43" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="B43" s="2" t="s">
+      <c r="C43" s="2" t="s">
         <v>39</v>
-      </c>
-      <c r="C43" s="2" t="s">
-        <v>40</v>
       </c>
     </row>
     <row r="44" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -1441,7 +1442,7 @@
         <v>4</v>
       </c>
       <c r="C44" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="45" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -1452,7 +1453,7 @@
         <v>4</v>
       </c>
       <c r="C45" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="46" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -1463,7 +1464,7 @@
         <v>4</v>
       </c>
       <c r="C46" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="47" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -1474,7 +1475,7 @@
         <v>4</v>
       </c>
       <c r="C47" s="2" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
     </row>
     <row r="48" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -1485,7 +1486,7 @@
         <v>4</v>
       </c>
       <c r="C48" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="49" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -1496,7 +1497,7 @@
         <v>4</v>
       </c>
       <c r="C49" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="50" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -1507,7 +1508,7 @@
         <v>4</v>
       </c>
       <c r="C50" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="51" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -1518,7 +1519,7 @@
         <v>4</v>
       </c>
       <c r="C51" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="52" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -1529,7 +1530,7 @@
         <v>4</v>
       </c>
       <c r="C52" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="53" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -1540,7 +1541,7 @@
         <v>4</v>
       </c>
       <c r="C53" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="54" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -1562,7 +1563,7 @@
         <v>4</v>
       </c>
       <c r="C55" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="56" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -1573,7 +1574,7 @@
         <v>4</v>
       </c>
       <c r="C56" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="57" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -1584,7 +1585,7 @@
         <v>4</v>
       </c>
       <c r="C57" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="58" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -1595,7 +1596,7 @@
         <v>4</v>
       </c>
       <c r="C58" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="59" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -1606,7 +1607,7 @@
         <v>4</v>
       </c>
       <c r="C59" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="60" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -1617,7 +1618,7 @@
         <v>4</v>
       </c>
       <c r="C60" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="61" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -1628,62 +1629,62 @@
         <v>4</v>
       </c>
       <c r="C61" s="2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="62" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A62" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="B62" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="B62" s="2" t="s">
+      <c r="C62" s="2" t="s">
         <v>55</v>
-      </c>
-      <c r="C62" s="2" t="s">
-        <v>56</v>
       </c>
     </row>
     <row r="63" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A63" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="B63" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="B63" s="2" t="s">
-        <v>53</v>
-      </c>
       <c r="C63" s="2" t="s">
-        <v>184</v>
+        <v>177</v>
       </c>
     </row>
     <row r="64" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A64" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="B64" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="B64" s="2" t="s">
+      <c r="C64" s="2" t="s">
         <v>50</v>
-      </c>
-      <c r="C64" s="2" t="s">
-        <v>51</v>
       </c>
     </row>
     <row r="65" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A65" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="B65" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="B65" s="2" t="s">
+      <c r="C65" s="2" t="s">
         <v>46</v>
-      </c>
-      <c r="C65" s="2" t="s">
-        <v>47</v>
       </c>
     </row>
     <row r="66" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A66" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B66" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="B66" s="2" t="s">
-        <v>21</v>
-      </c>
       <c r="C66" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="67" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -1694,7 +1695,7 @@
         <v>4</v>
       </c>
       <c r="C67" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="68" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -1705,7 +1706,7 @@
         <v>4</v>
       </c>
       <c r="C68" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="69" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -1716,7 +1717,7 @@
         <v>4</v>
       </c>
       <c r="C69" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="70" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -1727,7 +1728,7 @@
         <v>4</v>
       </c>
       <c r="C70" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="71" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -1738,7 +1739,7 @@
         <v>4</v>
       </c>
       <c r="C71" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="72" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -1749,7 +1750,7 @@
         <v>4</v>
       </c>
       <c r="C72" s="2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="73" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -1760,7 +1761,7 @@
         <v>4</v>
       </c>
       <c r="C73" s="2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="74" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -1771,40 +1772,40 @@
         <v>8</v>
       </c>
       <c r="C74" s="2" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="75" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A75" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="B75" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="B75" s="2" t="s">
+      <c r="C75" s="2" t="s">
         <v>63</v>
-      </c>
-      <c r="C75" s="2" t="s">
-        <v>64</v>
       </c>
     </row>
     <row r="76" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A76" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="B76" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="B76" s="2" t="s">
-        <v>67</v>
-      </c>
       <c r="C76" s="6" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
     </row>
     <row r="77" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A77" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B77" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="B77" s="2" t="s">
-        <v>14</v>
-      </c>
       <c r="C77" s="2" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="78" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -1815,18 +1816,18 @@
         <v>4</v>
       </c>
       <c r="C78" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="79" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A79" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="B79" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="B79" s="2" t="s">
-        <v>69</v>
-      </c>
       <c r="C79" s="2" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
     </row>
     <row r="80" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -1837,7 +1838,7 @@
         <v>4</v>
       </c>
       <c r="C80" s="2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="81" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -1845,10 +1846,10 @@
         <v>6</v>
       </c>
       <c r="B81" s="2" t="s">
-        <v>91</v>
+        <v>4</v>
       </c>
       <c r="C81" s="2" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="82" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -1859,7 +1860,7 @@
         <v>4</v>
       </c>
       <c r="C82" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="83" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -1870,40 +1871,40 @@
         <v>4</v>
       </c>
       <c r="C83" s="2" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="84" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A84" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="B84" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="B84" s="2" t="s">
+      <c r="C84" s="2" t="s">
         <v>79</v>
-      </c>
-      <c r="C84" s="2" t="s">
-        <v>80</v>
       </c>
     </row>
     <row r="85" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A85" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="B85" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="B85" s="2" t="s">
-        <v>67</v>
-      </c>
       <c r="C85" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="86" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A86" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B86" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="B86" s="2" t="s">
-        <v>26</v>
-      </c>
       <c r="C86" s="2" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="87" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -1925,7 +1926,7 @@
         <v>8</v>
       </c>
       <c r="C88" s="2" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="89" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -1969,7 +1970,7 @@
         <v>4</v>
       </c>
       <c r="C92" s="2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="93" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -1980,7 +1981,7 @@
         <v>4</v>
       </c>
       <c r="C93" s="2" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="94" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -1991,7 +1992,7 @@
         <v>4</v>
       </c>
       <c r="C94" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="95" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -2002,29 +2003,29 @@
         <v>4</v>
       </c>
       <c r="C95" s="2" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="96" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A96" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="B96" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="B96" s="2" t="s">
-        <v>63</v>
-      </c>
       <c r="C96" s="2" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="97" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A97" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="B97" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="B97" s="2" t="s">
+      <c r="C97" s="2" t="s">
         <v>84</v>
-      </c>
-      <c r="C97" s="2" t="s">
-        <v>85</v>
       </c>
     </row>
     <row r="98" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -2035,7 +2036,7 @@
         <v>4</v>
       </c>
       <c r="C98" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="99" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -2046,7 +2047,7 @@
         <v>4</v>
       </c>
       <c r="C99" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="100" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -2057,7 +2058,7 @@
         <v>4</v>
       </c>
       <c r="C100" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="101" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -2068,7 +2069,7 @@
         <v>4</v>
       </c>
       <c r="C101" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="102" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -2079,7 +2080,7 @@
         <v>4</v>
       </c>
       <c r="C102" s="2" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="103" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -2090,7 +2091,7 @@
         <v>4</v>
       </c>
       <c r="C103" s="2" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="104" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -2101,7 +2102,7 @@
         <v>4</v>
       </c>
       <c r="C104" s="2" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="105" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -2112,7 +2113,7 @@
         <v>4</v>
       </c>
       <c r="C105" s="2" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="106" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -2123,29 +2124,29 @@
         <v>4</v>
       </c>
       <c r="C106" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="107" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A107" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="B107" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="B107" s="2" t="s">
+      <c r="C107" s="2" t="s">
         <v>39</v>
-      </c>
-      <c r="C107" s="2" t="s">
-        <v>40</v>
       </c>
     </row>
     <row r="108" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A108" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="B108" s="2" t="s">
         <v>88</v>
       </c>
-      <c r="B108" s="2" t="s">
+      <c r="C108" s="2" t="s">
         <v>89</v>
-      </c>
-      <c r="C108" s="2" t="s">
-        <v>90</v>
       </c>
     </row>
     <row r="109" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -2156,29 +2157,29 @@
         <v>4</v>
       </c>
       <c r="C109" s="2" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="110" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A110" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="B110" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="B110" s="2" t="s">
-        <v>63</v>
-      </c>
       <c r="C110" s="2" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="111" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A111" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="B111" s="2" t="s">
         <v>88</v>
       </c>
-      <c r="B111" s="2" t="s">
+      <c r="C111" s="2" t="s">
         <v>89</v>
-      </c>
-      <c r="C111" s="2" t="s">
-        <v>90</v>
       </c>
     </row>
     <row r="112" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -2189,18 +2190,18 @@
         <v>4</v>
       </c>
       <c r="C112" s="2" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="113" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A113" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="B113" s="2" t="s">
         <v>88</v>
       </c>
-      <c r="B113" s="2" t="s">
-        <v>89</v>
-      </c>
       <c r="C113" s="2" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="114" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -2211,7 +2212,7 @@
         <v>4</v>
       </c>
       <c r="C114" s="2" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="115" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -2222,7 +2223,7 @@
         <v>4</v>
       </c>
       <c r="C115" s="2" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="116" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -2233,18 +2234,18 @@
         <v>4</v>
       </c>
       <c r="C116" s="2" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="117" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A117" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="B117" s="2" t="s">
         <v>88</v>
       </c>
-      <c r="B117" s="2" t="s">
+      <c r="C117" s="2" t="s">
         <v>89</v>
-      </c>
-      <c r="C117" s="2" t="s">
-        <v>90</v>
       </c>
     </row>
     <row r="118" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -2255,7 +2256,7 @@
         <v>4</v>
       </c>
       <c r="C118" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="119" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -2266,29 +2267,29 @@
         <v>4</v>
       </c>
       <c r="C119" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="120" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A120" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="B120" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="B120" s="2" t="s">
-        <v>84</v>
-      </c>
       <c r="C120" s="2" t="s">
-        <v>186</v>
+        <v>179</v>
       </c>
     </row>
     <row r="121" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A121" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="B121" s="2" t="s">
         <v>88</v>
       </c>
-      <c r="B121" s="2" t="s">
-        <v>89</v>
-      </c>
       <c r="C121" s="2" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="122" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -2299,7 +2300,7 @@
         <v>4</v>
       </c>
       <c r="C122" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="123" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -2310,7 +2311,7 @@
         <v>4</v>
       </c>
       <c r="C123" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="124" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -2321,7 +2322,7 @@
         <v>4</v>
       </c>
       <c r="C124" s="2" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="125" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -2332,7 +2333,7 @@
         <v>4</v>
       </c>
       <c r="C125" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="126" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -2343,7 +2344,7 @@
         <v>4</v>
       </c>
       <c r="C126" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="127" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -2365,7 +2366,7 @@
         <v>4</v>
       </c>
       <c r="C128" s="2" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="129" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -2376,7 +2377,7 @@
         <v>4</v>
       </c>
       <c r="C129" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="130" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -2387,7 +2388,7 @@
         <v>4</v>
       </c>
       <c r="C130" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="131" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -2398,7 +2399,7 @@
         <v>4</v>
       </c>
       <c r="C131" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="132" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -2409,7 +2410,7 @@
         <v>4</v>
       </c>
       <c r="C132" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="133" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -2420,7 +2421,7 @@
         <v>4</v>
       </c>
       <c r="C133" s="2" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="134" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -2431,7 +2432,7 @@
         <v>4</v>
       </c>
       <c r="C134" s="2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="135" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -2442,7 +2443,7 @@
         <v>4</v>
       </c>
       <c r="C135" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="136" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -2453,7 +2454,7 @@
         <v>4</v>
       </c>
       <c r="C136" s="2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="137" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -2464,7 +2465,7 @@
         <v>4</v>
       </c>
       <c r="C137" s="2" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="138" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -2475,7 +2476,7 @@
         <v>4</v>
       </c>
       <c r="C138" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="139" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -2486,7 +2487,7 @@
         <v>4</v>
       </c>
       <c r="C139" s="2" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="140" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -2497,7 +2498,7 @@
         <v>4</v>
       </c>
       <c r="C140" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="141" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -2508,7 +2509,7 @@
         <v>4</v>
       </c>
       <c r="C141" s="2" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
     </row>
     <row r="142" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -2519,7 +2520,7 @@
         <v>4</v>
       </c>
       <c r="C142" s="2" t="s">
-        <v>172</v>
+        <v>183</v>
       </c>
     </row>
     <row r="143" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -2530,7 +2531,7 @@
         <v>4</v>
       </c>
       <c r="C143" s="2" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
     </row>
     <row r="144" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -2541,7 +2542,7 @@
         <v>4</v>
       </c>
       <c r="C144" s="2" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="145" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -2552,7 +2553,7 @@
         <v>4</v>
       </c>
       <c r="C145" s="2" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
     </row>
     <row r="146" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -2563,7 +2564,7 @@
         <v>4</v>
       </c>
       <c r="C146" s="2" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
     </row>
     <row r="147" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -2574,7 +2575,7 @@
         <v>4</v>
       </c>
       <c r="C147" s="2" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
     </row>
     <row r="148" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -2596,7 +2597,7 @@
         <v>4</v>
       </c>
       <c r="C149" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="150" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -2607,7 +2608,7 @@
         <v>4</v>
       </c>
       <c r="C150" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="151" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -2618,7 +2619,7 @@
         <v>4</v>
       </c>
       <c r="C151" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="152" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -2629,7 +2630,7 @@
         <v>4</v>
       </c>
       <c r="C152" s="2" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="153" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -2640,7 +2641,7 @@
         <v>4</v>
       </c>
       <c r="C153" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="154" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -2662,7 +2663,7 @@
         <v>4</v>
       </c>
       <c r="C155" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="156" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -2673,7 +2674,7 @@
         <v>4</v>
       </c>
       <c r="C156" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="157" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -2684,7 +2685,7 @@
         <v>4</v>
       </c>
       <c r="C157" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="158" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -2695,7 +2696,7 @@
         <v>4</v>
       </c>
       <c r="C158" s="2" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="159" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -2706,7 +2707,7 @@
         <v>4</v>
       </c>
       <c r="C159" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="160" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -2717,7 +2718,7 @@
         <v>4</v>
       </c>
       <c r="C160" s="2" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="161" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -2728,7 +2729,7 @@
         <v>4</v>
       </c>
       <c r="C161" s="2" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
     </row>
     <row r="162" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -2739,7 +2740,7 @@
         <v>4</v>
       </c>
       <c r="C162" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="163" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -2750,7 +2751,7 @@
         <v>4</v>
       </c>
       <c r="C163" s="2" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="164" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -2761,7 +2762,7 @@
         <v>4</v>
       </c>
       <c r="C164" s="2" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="165" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -2772,7 +2773,7 @@
         <v>4</v>
       </c>
       <c r="C165" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="166" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -2783,7 +2784,7 @@
         <v>4</v>
       </c>
       <c r="C166" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="167" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -2794,7 +2795,7 @@
         <v>4</v>
       </c>
       <c r="C167" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="168" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -2805,7 +2806,7 @@
         <v>4</v>
       </c>
       <c r="C168" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="169" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -2816,7 +2817,7 @@
         <v>4</v>
       </c>
       <c r="C169" s="2" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
     </row>
     <row r="170" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -2838,7 +2839,7 @@
         <v>4</v>
       </c>
       <c r="C171" s="2" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="172" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -2849,7 +2850,7 @@
         <v>4</v>
       </c>
       <c r="C172" s="2" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="173" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -2860,7 +2861,7 @@
         <v>4</v>
       </c>
       <c r="C173" s="2" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="174" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -2871,7 +2872,7 @@
         <v>4</v>
       </c>
       <c r="C174" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="175" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -2882,7 +2883,7 @@
         <v>4</v>
       </c>
       <c r="C175" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="176" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -2893,7 +2894,7 @@
         <v>4</v>
       </c>
       <c r="C176" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="177" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -2904,7 +2905,7 @@
         <v>4</v>
       </c>
       <c r="C177" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="178" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -2915,7 +2916,7 @@
         <v>4</v>
       </c>
       <c r="C178" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="179" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -2926,7 +2927,7 @@
         <v>4</v>
       </c>
       <c r="C179" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="180" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -2937,7 +2938,7 @@
         <v>4</v>
       </c>
       <c r="C180" s="2" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
     </row>
     <row r="181" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -2948,7 +2949,7 @@
         <v>4</v>
       </c>
       <c r="C181" s="2" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="182" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -2959,7 +2960,7 @@
         <v>4</v>
       </c>
       <c r="C182" s="2" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
     </row>
     <row r="183" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -2970,7 +2971,7 @@
         <v>4</v>
       </c>
       <c r="C183" s="2" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="184" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -2981,7 +2982,7 @@
         <v>4</v>
       </c>
       <c r="C184" s="2" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="185" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -2992,7 +2993,7 @@
         <v>4</v>
       </c>
       <c r="C185" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="186" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -3003,7 +3004,7 @@
         <v>4</v>
       </c>
       <c r="C186" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="187" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -3014,7 +3015,7 @@
         <v>4</v>
       </c>
       <c r="C187" s="2" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="188" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -3025,7 +3026,7 @@
         <v>4</v>
       </c>
       <c r="C188" s="2" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="189" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -3036,7 +3037,7 @@
         <v>4</v>
       </c>
       <c r="C189" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="190" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -3047,7 +3048,7 @@
         <v>4</v>
       </c>
       <c r="C190" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="191" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -3058,7 +3059,7 @@
         <v>4</v>
       </c>
       <c r="C191" s="2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="192" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -3069,7 +3070,7 @@
         <v>4</v>
       </c>
       <c r="C192" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="193" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -3080,29 +3081,29 @@
         <v>4</v>
       </c>
       <c r="C193" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="194" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A194" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B194" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="B194" s="2" t="s">
-        <v>14</v>
-      </c>
       <c r="C194" s="2" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="195" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A195" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B195" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="B195" s="2" t="s">
-        <v>14</v>
-      </c>
       <c r="C195" s="2" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="196" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -3113,7 +3114,7 @@
         <v>4</v>
       </c>
       <c r="C196" s="2" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="197" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -3124,29 +3125,29 @@
         <v>4</v>
       </c>
       <c r="C197" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="198" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A198" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="B198" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="B198" s="2" t="s">
-        <v>39</v>
-      </c>
       <c r="C198" s="2" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
     </row>
     <row r="199" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A199" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="B199" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="B199" s="2" t="s">
-        <v>39</v>
-      </c>
       <c r="C199" s="2" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
     </row>
     <row r="200" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -3157,7 +3158,7 @@
         <v>4</v>
       </c>
       <c r="C200" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="201" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -3179,7 +3180,7 @@
         <v>4</v>
       </c>
       <c r="C202" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="203" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -3190,7 +3191,7 @@
         <v>4</v>
       </c>
       <c r="C203" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="204" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -3201,7 +3202,7 @@
         <v>4</v>
       </c>
       <c r="C204" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="205" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -3212,7 +3213,7 @@
         <v>4</v>
       </c>
       <c r="C205" s="2" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="206" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -3223,7 +3224,7 @@
         <v>4</v>
       </c>
       <c r="C206" s="2" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="207" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -3234,7 +3235,7 @@
         <v>4</v>
       </c>
       <c r="C207" s="2" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="208" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -3245,18 +3246,18 @@
         <v>4</v>
       </c>
       <c r="C208" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="209" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A209" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="B209" s="2" t="s">
         <v>122</v>
       </c>
-      <c r="B209" s="2" t="s">
-        <v>123</v>
-      </c>
       <c r="C209" s="2" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
     </row>
     <row r="210" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -3267,7 +3268,7 @@
         <v>4</v>
       </c>
       <c r="C210" s="2" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="211" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -3278,7 +3279,7 @@
         <v>4</v>
       </c>
       <c r="C211" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="212" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -3289,7 +3290,7 @@
         <v>4</v>
       </c>
       <c r="C212" s="2" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="213" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -3300,7 +3301,7 @@
         <v>4</v>
       </c>
       <c r="C213" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="214" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -3311,7 +3312,7 @@
         <v>4</v>
       </c>
       <c r="C214" s="2" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="215" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -3322,7 +3323,7 @@
         <v>4</v>
       </c>
       <c r="C215" s="2" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="216" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -3333,7 +3334,7 @@
         <v>4</v>
       </c>
       <c r="C216" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="217" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -3344,7 +3345,7 @@
         <v>4</v>
       </c>
       <c r="C217" s="2" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="218" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -3355,7 +3356,7 @@
         <v>4</v>
       </c>
       <c r="C218" s="2" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="219" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -3366,7 +3367,7 @@
         <v>4</v>
       </c>
       <c r="C219" s="2" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="220" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -3377,7 +3378,7 @@
         <v>4</v>
       </c>
       <c r="C220" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="221" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -3388,7 +3389,7 @@
         <v>4</v>
       </c>
       <c r="C221" s="2" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="222" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -3410,7 +3411,7 @@
         <v>4</v>
       </c>
       <c r="C223" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="224" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -3421,18 +3422,18 @@
         <v>8</v>
       </c>
       <c r="C224" s="2" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
     </row>
     <row r="225" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A225" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="B225" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="B225" s="2" t="s">
-        <v>84</v>
-      </c>
       <c r="C225" s="2" t="s">
-        <v>131</v>
+        <v>180</v>
       </c>
     </row>
     <row r="226" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -3443,7 +3444,7 @@
         <v>4</v>
       </c>
       <c r="C226" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="227" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -3454,7 +3455,7 @@
         <v>4</v>
       </c>
       <c r="C227" s="2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="228" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -3465,18 +3466,18 @@
         <v>4</v>
       </c>
       <c r="C228" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="229" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A229" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="B229" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="B229" s="2" t="s">
-        <v>84</v>
-      </c>
       <c r="C229" s="2" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
     </row>
     <row r="230" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -3487,18 +3488,18 @@
         <v>4</v>
       </c>
       <c r="C230" s="2" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
     </row>
     <row r="231" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A231" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="B231" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="B231" s="2" t="s">
-        <v>180</v>
-      </c>
       <c r="C231" s="2" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
     </row>
     <row r="232" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -3509,7 +3510,7 @@
         <v>4</v>
       </c>
       <c r="C232" s="2" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
     </row>
     <row r="233" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -3517,10 +3518,10 @@
         <v>10</v>
       </c>
       <c r="B233" s="2" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="C233" s="2" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
     </row>
     <row r="234" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -3531,7 +3532,7 @@
         <v>4</v>
       </c>
       <c r="C234" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="235" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -3542,7 +3543,7 @@
         <v>4</v>
       </c>
       <c r="C235" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="236" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -3553,7 +3554,7 @@
         <v>4</v>
       </c>
       <c r="C236" s="2" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="237" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -3564,18 +3565,18 @@
         <v>4</v>
       </c>
       <c r="C237" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="238" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A238" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="B238" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="B238" s="2" t="s">
-        <v>84</v>
-      </c>
       <c r="C238" s="2" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
     </row>
     <row r="239" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -3583,10 +3584,10 @@
         <v>7</v>
       </c>
       <c r="B239" s="2" t="s">
-        <v>181</v>
+        <v>8</v>
       </c>
       <c r="C239" s="2" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
     </row>
     <row r="240" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -3608,18 +3609,18 @@
         <v>4</v>
       </c>
       <c r="C241" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="242" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A242" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="B242" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="B242" s="2" t="s">
-        <v>84</v>
-      </c>
       <c r="C242" s="2" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
     </row>
     <row r="243" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -3630,7 +3631,7 @@
         <v>4</v>
       </c>
       <c r="C243" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="244" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -3652,7 +3653,7 @@
         <v>4</v>
       </c>
       <c r="C245" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="246" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -3674,7 +3675,7 @@
         <v>4</v>
       </c>
       <c r="C247" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="248" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -3685,7 +3686,7 @@
         <v>4</v>
       </c>
       <c r="C248" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="249" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -3696,7 +3697,7 @@
         <v>4</v>
       </c>
       <c r="C249" s="2" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
     </row>
     <row r="250" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -3707,7 +3708,7 @@
         <v>4</v>
       </c>
       <c r="C250" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="251" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -3718,7 +3719,7 @@
         <v>4</v>
       </c>
       <c r="C251" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="252" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -3729,7 +3730,7 @@
         <v>4</v>
       </c>
       <c r="C252" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="253" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -3740,7 +3741,7 @@
         <v>4</v>
       </c>
       <c r="C253" s="2" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
     </row>
     <row r="254" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -3751,7 +3752,7 @@
         <v>4</v>
       </c>
       <c r="C254" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="255" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -3773,7 +3774,7 @@
         <v>4</v>
       </c>
       <c r="C256" s="2" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
     </row>
     <row r="257" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -3784,18 +3785,18 @@
         <v>4</v>
       </c>
       <c r="C257" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="258" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A258" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B258" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="B258" s="2" t="s">
-        <v>14</v>
-      </c>
       <c r="C258" s="2" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="259" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -3803,10 +3804,10 @@
         <v>7</v>
       </c>
       <c r="B259" s="2" t="s">
-        <v>181</v>
+        <v>8</v>
       </c>
       <c r="C259" s="2" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
     </row>
     <row r="260" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -3817,7 +3818,7 @@
         <v>4</v>
       </c>
       <c r="C260" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="261" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -3828,7 +3829,7 @@
         <v>4</v>
       </c>
       <c r="C261" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="262" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -3839,18 +3840,18 @@
         <v>4</v>
       </c>
       <c r="C262" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="263" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A263" s="2" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="B263" s="2" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="C263" s="2" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
     </row>
     <row r="264" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -3861,7 +3862,7 @@
         <v>4</v>
       </c>
       <c r="C264" s="2" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
     </row>
     <row r="265" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -3872,7 +3873,7 @@
         <v>4</v>
       </c>
       <c r="C265" s="2" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
     </row>
     <row r="266" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -3883,7 +3884,7 @@
         <v>4</v>
       </c>
       <c r="C266" s="2" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
     </row>
     <row r="267" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -3894,7 +3895,7 @@
         <v>4</v>
       </c>
       <c r="C267" s="2" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="268" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -3905,7 +3906,7 @@
         <v>4</v>
       </c>
       <c r="C268" s="2" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
     </row>
     <row r="269" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -3916,7 +3917,7 @@
         <v>4</v>
       </c>
       <c r="C269" s="2" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="270" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -3938,7 +3939,7 @@
         <v>4</v>
       </c>
       <c r="C271" s="2" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
     </row>
     <row r="272" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -3954,13 +3955,13 @@
     </row>
     <row r="273" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A273" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B273" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="B273" s="2" t="s">
-        <v>32</v>
-      </c>
       <c r="C273" s="2" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
     </row>
     <row r="274" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -3971,18 +3972,18 @@
         <v>4</v>
       </c>
       <c r="C274" s="2" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="275" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A275" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B275" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="B275" s="2" t="s">
-        <v>14</v>
-      </c>
       <c r="C275" s="2" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
     </row>
     <row r="276" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -3993,7 +3994,7 @@
         <v>4</v>
       </c>
       <c r="C276" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="277" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -4004,7 +4005,7 @@
         <v>4</v>
       </c>
       <c r="C277" s="2" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
     </row>
     <row r="278" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -4015,7 +4016,7 @@
         <v>4</v>
       </c>
       <c r="C278" s="2" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="279" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -4026,7 +4027,7 @@
         <v>4</v>
       </c>
       <c r="C279" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="280" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -4037,7 +4038,7 @@
         <v>4</v>
       </c>
       <c r="C280" s="2" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
     </row>
     <row r="281" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -4048,7 +4049,7 @@
         <v>4</v>
       </c>
       <c r="C281" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="282" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -4059,7 +4060,7 @@
         <v>4</v>
       </c>
       <c r="C282" s="2" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
     </row>
     <row r="283" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -4070,7 +4071,7 @@
         <v>4</v>
       </c>
       <c r="C283" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="284" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -4081,7 +4082,7 @@
         <v>4</v>
       </c>
       <c r="C284" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="285" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -4092,7 +4093,7 @@
         <v>4</v>
       </c>
       <c r="C285" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="286" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -4103,7 +4104,7 @@
         <v>4</v>
       </c>
       <c r="C286" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="287" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -4114,7 +4115,7 @@
         <v>4</v>
       </c>
       <c r="C287" s="2" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
     </row>
     <row r="288" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -4125,7 +4126,7 @@
         <v>4</v>
       </c>
       <c r="C288" s="2" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
     </row>
     <row r="289" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -4136,29 +4137,29 @@
         <v>4</v>
       </c>
       <c r="C289" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="290" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A290" s="2" t="s">
+        <v>148</v>
+      </c>
+      <c r="B290" s="2" t="s">
+        <v>149</v>
+      </c>
+      <c r="C290" s="2" t="s">
         <v>150</v>
-      </c>
-      <c r="B290" s="2" t="s">
-        <v>151</v>
-      </c>
-      <c r="C290" s="2" t="s">
-        <v>152</v>
       </c>
     </row>
     <row r="291" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A291" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="B291" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="B291" s="2" t="s">
-        <v>84</v>
-      </c>
       <c r="C291" s="2" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
     </row>
     <row r="292" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -4169,7 +4170,7 @@
         <v>4</v>
       </c>
       <c r="C292" s="2" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="293" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -4180,7 +4181,7 @@
         <v>4</v>
       </c>
       <c r="C293" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="294" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -4191,7 +4192,7 @@
         <v>4</v>
       </c>
       <c r="C294" s="2" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="295" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -4202,7 +4203,7 @@
         <v>4</v>
       </c>
       <c r="C295" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="296" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -4213,7 +4214,7 @@
         <v>4</v>
       </c>
       <c r="C296" s="2" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="297" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -4224,7 +4225,7 @@
         <v>4</v>
       </c>
       <c r="C297" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="298" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -4235,7 +4236,7 @@
         <v>4</v>
       </c>
       <c r="C298" s="2" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="299" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -4246,7 +4247,7 @@
         <v>4</v>
       </c>
       <c r="C299" s="2" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
     </row>
     <row r="300" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25"/>
@@ -24719,7 +24720,7 @@
       <c r="C11407" s="7"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:C9078"/>
+  <autoFilter ref="A1:C9078" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
 </worksheet>

</xml_diff>